<commit_message>
codigo de barras add
</commit_message>
<xml_diff>
--- a/cobranca.xlsx
+++ b/cobranca.xlsx
@@ -25,7 +25,7 @@
     <t>Telefone</t>
   </si>
   <si>
-    <t>Telefone Celular</t>
+    <t>codigo de barras</t>
   </si>
 </sst>
 </file>
@@ -69,10 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +381,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +405,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -467,5 +469,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>